<commit_message>
When do ScreenShot or ExecuteSQL Then you can show message.
</commit_message>
<xml_diff>
--- a/EvidenceTemplate.xlsx
+++ b/EvidenceTemplate.xlsx
@@ -74,11 +74,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -380,25 +381,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="2.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.75" style="2" customWidth="1"/>
     <col min="3" max="3" width="2.875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="3"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B64" s="2"/>
+      <c r="B64" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -410,23 +413,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="2.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="3"/>
+    <col min="2" max="2" width="2.75" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B64" s="2"/>
+      <c r="B64" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
Create PaperTester class. Create exexute file. Add error handling process.
</commit_message>
<xml_diff>
--- a/EvidenceTemplate.xlsx
+++ b/EvidenceTemplate.xlsx
@@ -383,9 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -413,9 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>